<commit_message>
Corrections were made to the Japanese version.
</commit_message>
<xml_diff>
--- a/en/Sample_Project/Source_Code/climan-project/src/test/java/com/nablarch/example/climan/rest/client/ClientActionTest.xlsx
+++ b/en/Sample_Project/Source_Code/climan-project/src/test/java/com/nablarch/example/climan/rest/client/ClientActionTest.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5389FAD3-91E2-4011-AE54-46999586BF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0525C6-D42C-409D-B242-B344DA3C6D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FCC07A5D-5645-46B3-BC0B-1ABBDDE24C74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCC07A5D-5645-46B3-BC0B-1ABBDDE24C74}"/>
   </bookViews>
   <sheets>
     <sheet name="setUpDb" sheetId="1" r:id="rId1"/>
-    <sheet name="testFindUnderUpperLimit" sheetId="4" r:id="rId2"/>
-    <sheet name="testFindOverUpperLimit" sheetId="3" r:id="rId3"/>
+    <sheet name="testFindNoClients" sheetId="5" r:id="rId2"/>
+    <sheet name="testShowWithEmptyClientTable" sheetId="6" r:id="rId3"/>
+    <sheet name="testFindIndustryCodeNoClients" sheetId="7" r:id="rId4"/>
+    <sheet name="testFindCodeAndNameUpperLimit" sheetId="8" r:id="rId5"/>
+    <sheet name="testFindOverUpperLimit" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6036" uniqueCount="2017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6066" uniqueCount="2017">
   <si>
     <t>CLIENT_ID</t>
   </si>
@@ -6113,20 +6116,20 @@
     <font>
       <sz val="17"/>
       <color indexed="9"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color indexed="9"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -6514,7 +6517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B653223-24B4-4336-9A7B-ADEB889ABA54}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
@@ -6633,7 +6636,230 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA35B3DB-149A-4F52-BF71-026E7882D85D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FD53BC-A36C-43D1-9E3C-270227781B9B}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="13.25" style="7"/>
+    <col min="2" max="2" width="33.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="13.25" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D433D5-35E1-4436-B8F9-2297528F2F70}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="13.25" style="7"/>
+    <col min="2" max="2" width="33.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="13.25" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE669A41-ED44-4773-B45A-F4ECE45DAC8B}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="13.25" style="7"/>
+    <col min="2" max="2" width="33.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="13.25" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5C464F-A84D-4B16-A81A-7423DF3B4D1F}">
   <dimension ref="A1:J1004"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -17688,7 +17914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51B27E0-8AD5-4212-B9A3-4B56C2C9A649}">
   <dimension ref="A1:J1005"/>
   <sheetViews>

</xml_diff>

<commit_message>
英語版 junit test (#140)
* Corrections were made to the Japanese version.

* Corrections were made to the Japanese version.

* コメントの脱字修正

* Fixed missing text in comments

* Corrections were made to the Japanese version.

* Corrections were made to the Japanese version.
</commit_message>
<xml_diff>
--- a/en/Sample_Project/Source_Code/climan-project/src/test/java/com/nablarch/example/climan/rest/client/ClientActionTest.xlsx
+++ b/en/Sample_Project/Source_Code/climan-project/src/test/java/com/nablarch/example/climan/rest/client/ClientActionTest.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5389FAD3-91E2-4011-AE54-46999586BF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0525C6-D42C-409D-B242-B344DA3C6D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FCC07A5D-5645-46B3-BC0B-1ABBDDE24C74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCC07A5D-5645-46B3-BC0B-1ABBDDE24C74}"/>
   </bookViews>
   <sheets>
     <sheet name="setUpDb" sheetId="1" r:id="rId1"/>
-    <sheet name="testFindUnderUpperLimit" sheetId="4" r:id="rId2"/>
-    <sheet name="testFindOverUpperLimit" sheetId="3" r:id="rId3"/>
+    <sheet name="testFindNoClients" sheetId="5" r:id="rId2"/>
+    <sheet name="testShowWithEmptyClientTable" sheetId="6" r:id="rId3"/>
+    <sheet name="testFindIndustryCodeNoClients" sheetId="7" r:id="rId4"/>
+    <sheet name="testFindCodeAndNameUpperLimit" sheetId="8" r:id="rId5"/>
+    <sheet name="testFindOverUpperLimit" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6036" uniqueCount="2017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6066" uniqueCount="2017">
   <si>
     <t>CLIENT_ID</t>
   </si>
@@ -6113,20 +6116,20 @@
     <font>
       <sz val="17"/>
       <color indexed="9"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color indexed="9"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -6514,7 +6517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B653223-24B4-4336-9A7B-ADEB889ABA54}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
@@ -6633,7 +6636,230 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA35B3DB-149A-4F52-BF71-026E7882D85D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FD53BC-A36C-43D1-9E3C-270227781B9B}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="13.25" style="7"/>
+    <col min="2" max="2" width="33.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="13.25" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D433D5-35E1-4436-B8F9-2297528F2F70}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="13.25" style="7"/>
+    <col min="2" max="2" width="33.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="13.25" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE669A41-ED44-4773-B45A-F4ECE45DAC8B}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="13.25" style="7"/>
+    <col min="2" max="2" width="33.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="13.25" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5C464F-A84D-4B16-A81A-7423DF3B4D1F}">
   <dimension ref="A1:J1004"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -17688,7 +17914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51B27E0-8AD5-4212-B9A3-4B56C2C9A649}">
   <dimension ref="A1:J1005"/>
   <sheetViews>

</xml_diff>